<commit_message>
+ Fixed missing interface marker on ProxyHTTPEncoder. + Ran through manual integration testing. + Updated release sheet and added new release sheet.
</commit_message>
<xml_diff>
--- a/ReleaseCheckSheet.xlsx
+++ b/ReleaseCheckSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>MDACSHTTPServer Release Checkoff</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>Commit</t>
+  </si>
+  <si>
+    <t>Was the build performed using a release configuration?</t>
+  </si>
+  <si>
+    <t>Were all tests performed using the release configuration?</t>
+  </si>
+  <si>
+    <t>Was the test performed with HTTP pipelining fully enabled?</t>
+  </si>
+  <si>
+    <t>Was version properly marked in NUGET configuration before commit?</t>
+  </si>
+  <si>
+    <t>Has version in project configuration and NUGET config been updated?</t>
   </si>
 </sst>
 </file>
@@ -96,9 +111,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -418,32 +439,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -461,7 +485,7 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -544,17 +568,87 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B10:J10"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
+  <mergeCells count="15">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="B10:J10"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="B12:J12"/>
     <mergeCell ref="B9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>